<commit_message>
more tests, comparing eurusd vs gbpnzd
</commit_message>
<xml_diff>
--- a/TestSet32.xlsx
+++ b/TestSet32.xlsx
@@ -410,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:D13"/>
+    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,7 +476,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="4" t="str">
-        <f>$B$3&amp;" Both "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml"&amp;" "&amp;$B$2&amp;"DataShape"&amp;$B6&amp;".xml "&amp;$B$2&amp;"trainDataSet"&amp;$C6&amp;".xml "&amp;$B$2&amp;"Engine"&amp;$A6&amp;".xml"</f>
+        <f t="shared" ref="D6:D21" si="0">$B$3&amp;" Both "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml"&amp;" "&amp;$B$2&amp;"DataShape"&amp;$B6&amp;".xml "&amp;$B$2&amp;"trainDataSet"&amp;$C6&amp;".xml "&amp;$B$2&amp;"Engine"&amp;$A6&amp;".xml"</f>
         <v>zzz Both 32 Config/32/Client.xml Config/32/DataShape0.xml Config/32/trainDataSet1.xml Config/32/Engine1.xml</v>
       </c>
     </row>
@@ -491,7 +491,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="4" t="str">
-        <f>$B$3&amp;" Both "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml"&amp;" "&amp;$B$2&amp;"DataShape"&amp;$B7&amp;".xml "&amp;$B$2&amp;"trainDataSet"&amp;$C7&amp;".xml "&amp;$B$2&amp;"Engine"&amp;$A7&amp;".xml"</f>
+        <f t="shared" si="0"/>
         <v>zzz Both 32 Config/32/Client.xml Config/32/DataShape0.xml Config/32/trainDataSet1.xml Config/32/Engine2.xml</v>
       </c>
     </row>
@@ -506,7 +506,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="4" t="str">
-        <f>$B$3&amp;" Both "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml"&amp;" "&amp;$B$2&amp;"DataShape"&amp;$B8&amp;".xml "&amp;$B$2&amp;"trainDataSet"&amp;$C8&amp;".xml "&amp;$B$2&amp;"Engine"&amp;$A8&amp;".xml"</f>
+        <f t="shared" si="0"/>
         <v>zzz Both 32 Config/32/Client.xml Config/32/DataShape0.xml Config/32/trainDataSet1.xml Config/32/Engine3.xml</v>
       </c>
     </row>
@@ -521,7 +521,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="4" t="str">
-        <f>$B$3&amp;" Both "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml"&amp;" "&amp;$B$2&amp;"DataShape"&amp;$B9&amp;".xml "&amp;$B$2&amp;"trainDataSet"&amp;$C9&amp;".xml "&amp;$B$2&amp;"Engine"&amp;$A9&amp;".xml"</f>
+        <f t="shared" si="0"/>
         <v>zzz Both 32 Config/32/Client.xml Config/32/DataShape0.xml Config/32/trainDataSet1.xml Config/32/Engine4.xml</v>
       </c>
     </row>
@@ -536,7 +536,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="4" t="str">
-        <f>$B$3&amp;" Both "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml"&amp;" "&amp;$B$2&amp;"DataShape"&amp;$B10&amp;".xml "&amp;$B$2&amp;"trainDataSet"&amp;$C10&amp;".xml "&amp;$B$2&amp;"Engine"&amp;$A10&amp;".xml"</f>
+        <f t="shared" si="0"/>
         <v>zzz Both 32 Config/32/Client.xml Config/32/DataShape1.xml Config/32/trainDataSet1.xml Config/32/Engine1.xml</v>
       </c>
     </row>
@@ -551,7 +551,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="4" t="str">
-        <f>$B$3&amp;" Both "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml"&amp;" "&amp;$B$2&amp;"DataShape"&amp;$B11&amp;".xml "&amp;$B$2&amp;"trainDataSet"&amp;$C11&amp;".xml "&amp;$B$2&amp;"Engine"&amp;$A11&amp;".xml"</f>
+        <f t="shared" si="0"/>
         <v>zzz Both 32 Config/32/Client.xml Config/32/DataShape1.xml Config/32/trainDataSet1.xml Config/32/Engine2.xml</v>
       </c>
     </row>
@@ -566,7 +566,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="4" t="str">
-        <f>$B$3&amp;" Both "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml"&amp;" "&amp;$B$2&amp;"DataShape"&amp;$B12&amp;".xml "&amp;$B$2&amp;"trainDataSet"&amp;$C12&amp;".xml "&amp;$B$2&amp;"Engine"&amp;$A12&amp;".xml"</f>
+        <f t="shared" si="0"/>
         <v>zzz Both 32 Config/32/Client.xml Config/32/DataShape1.xml Config/32/trainDataSet1.xml Config/32/Engine3.xml</v>
       </c>
     </row>
@@ -581,68 +581,128 @@
         <v>1</v>
       </c>
       <c r="D13" s="4" t="str">
-        <f>$B$3&amp;" Both "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml"&amp;" "&amp;$B$2&amp;"DataShape"&amp;$B13&amp;".xml "&amp;$B$2&amp;"trainDataSet"&amp;$C13&amp;".xml "&amp;$B$2&amp;"Engine"&amp;$A13&amp;".xml"</f>
+        <f t="shared" si="0"/>
         <v>zzz Both 32 Config/32/Client.xml Config/32/DataShape1.xml Config/32/trainDataSet1.xml Config/32/Engine4.xml</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
+      <c r="A14" s="4">
+        <v>1</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="4" t="str">
-        <f>$B$3&amp;" Both "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml"&amp;" "&amp;$B$2&amp;"DataShape"&amp;$B14&amp;".xml "&amp;$B$2&amp;"trainDataSet"&amp;$C14&amp;".xml "&amp;$B$2&amp;"Engine"&amp;$A14&amp;".xml"</f>
-        <v>zzz Both 32 Config/32/Client.xml Config/32/DataShape2.xml Config/32/trainDataSet1.xml Config/32/Engine1.xml</v>
+        <f t="shared" si="0"/>
+        <v>zzz Both 32 Config/32/Client.xml Config/32/DataShape0.xml Config/32/trainDataSet2.xml Config/32/Engine1.xml</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
+      <c r="A15" s="4">
+        <v>2</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="4" t="str">
-        <f>$B$3&amp;" Both "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml"&amp;" "&amp;$B$2&amp;"DataShape"&amp;$B15&amp;".xml "&amp;$B$2&amp;"trainDataSet"&amp;$C15&amp;".xml "&amp;$B$2&amp;"Engine"&amp;$A15&amp;".xml"</f>
-        <v>zzz Both 32 Config/32/Client.xml Config/32/DataShape2.xml Config/32/trainDataSet1.xml Config/32/Engine2.xml</v>
+        <f t="shared" si="0"/>
+        <v>zzz Both 32 Config/32/Client.xml Config/32/DataShape0.xml Config/32/trainDataSet2.xml Config/32/Engine2.xml</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="4">
         <v>3</v>
       </c>
-      <c r="B16">
-        <v>2</v>
+      <c r="B16" s="4">
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="4" t="str">
-        <f>$B$3&amp;" Both "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml"&amp;" "&amp;$B$2&amp;"DataShape"&amp;$B16&amp;".xml "&amp;$B$2&amp;"trainDataSet"&amp;$C16&amp;".xml "&amp;$B$2&amp;"Engine"&amp;$A16&amp;".xml"</f>
-        <v>zzz Both 32 Config/32/Client.xml Config/32/DataShape2.xml Config/32/trainDataSet1.xml Config/32/Engine3.xml</v>
+        <f t="shared" si="0"/>
+        <v>zzz Both 32 Config/32/Client.xml Config/32/DataShape0.xml Config/32/trainDataSet2.xml Config/32/Engine3.xml</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="A17" s="4">
         <v>4</v>
       </c>
-      <c r="B17">
-        <v>2</v>
+      <c r="B17" s="4">
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="4" t="str">
-        <f>$B$3&amp;" Both "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml"&amp;" "&amp;$B$2&amp;"DataShape"&amp;$B17&amp;".xml "&amp;$B$2&amp;"trainDataSet"&amp;$C17&amp;".xml "&amp;$B$2&amp;"Engine"&amp;$A17&amp;".xml"</f>
-        <v>zzz Both 32 Config/32/Client.xml Config/32/DataShape2.xml Config/32/trainDataSet1.xml Config/32/Engine4.xml</v>
+        <f t="shared" si="0"/>
+        <v>zzz Both 32 Config/32/Client.xml Config/32/DataShape0.xml Config/32/trainDataSet2.xml Config/32/Engine4.xml</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>1</v>
+      </c>
+      <c r="B18" s="4">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>zzz Both 32 Config/32/Client.xml Config/32/DataShape1.xml Config/32/trainDataSet2.xml Config/32/Engine1.xml</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>2</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>zzz Both 32 Config/32/Client.xml Config/32/DataShape1.xml Config/32/trainDataSet2.xml Config/32/Engine2.xml</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>3</v>
+      </c>
+      <c r="B20" s="4">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>zzz Both 32 Config/32/Client.xml Config/32/DataShape1.xml Config/32/trainDataSet2.xml Config/32/Engine3.xml</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>4</v>
+      </c>
+      <c r="B21" s="4">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>zzz Both 32 Config/32/Client.xml Config/32/DataShape1.xml Config/32/trainDataSet2.xml Config/32/Engine4.xml</v>
       </c>
     </row>
   </sheetData>
@@ -659,10 +719,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -756,227 +816,202 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
-        <v>8624</v>
+        <v>2052</v>
       </c>
       <c r="C6" s="4" t="str">
-        <f t="shared" ref="C6:C14" si="1">$B$3&amp;" Infer "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml"&amp;" "&amp;$B$2&amp;"trainDataSet"&amp;$C$3&amp;".xml "&amp;$A6</f>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/trainDataSet1.xml 8624</v>
+        <f t="shared" ref="C6:C13" si="1">$B$3&amp;" Infer "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml"&amp;" "&amp;$B$2&amp;"trainDataSet"&amp;$C$3&amp;".xml "&amp;$A6</f>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/trainDataSet1.xml 2052</v>
       </c>
       <c r="D6" s="3" t="str">
-        <f t="shared" ref="D6:G14" si="2">$B$3&amp;" Infer "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml "&amp;$B$2&amp;"inferDataSet"&amp;D$3&amp;".xml "&amp;$A6</f>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet1.xml 8624</v>
+        <f t="shared" ref="D6:G13" si="2">$B$3&amp;" Infer "&amp;$B$1&amp;" "&amp;$B$2&amp;"Client.xml "&amp;$B$2&amp;"inferDataSet"&amp;D$3&amp;".xml "&amp;$A6</f>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet1.xml 2052</v>
       </c>
       <c r="E6" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet2.xml 8624</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet2.xml 2052</v>
       </c>
       <c r="F6" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet3.xml 8624</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet3.xml 2052</v>
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet4.xml 8624</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet4.xml 2052</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
-        <v>13192</v>
+        <v>12000</v>
       </c>
       <c r="C7" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/trainDataSet1.xml 13192</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/trainDataSet1.xml 12000</v>
       </c>
       <c r="D7" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet1.xml 13192</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet1.xml 12000</v>
       </c>
       <c r="E7" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet2.xml 13192</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet2.xml 12000</v>
       </c>
       <c r="F7" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet3.xml 13192</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet3.xml 12000</v>
       </c>
       <c r="G7" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet4.xml 13192</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet4.xml 12000</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
-        <v>3088</v>
+        <v>12088</v>
       </c>
       <c r="C8" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/trainDataSet1.xml 3088</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/trainDataSet1.xml 12088</v>
       </c>
       <c r="D8" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet1.xml 3088</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet1.xml 12088</v>
       </c>
       <c r="E8" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet2.xml 3088</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet2.xml 12088</v>
       </c>
       <c r="F8" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet3.xml 3088</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet3.xml 12088</v>
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet4.xml 3088</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet4.xml 12088</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
-        <v>3416</v>
+        <v>2292</v>
       </c>
       <c r="C9" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/trainDataSet1.xml 3416</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/trainDataSet1.xml 2292</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet1.xml 3416</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet1.xml 2292</v>
       </c>
       <c r="E9" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet2.xml 3416</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet2.xml 2292</v>
       </c>
       <c r="F9" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet3.xml 3416</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet3.xml 2292</v>
       </c>
       <c r="G9" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet4.xml 3416</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet4.xml 2292</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
-        <v>7660</v>
+        <v>14608</v>
       </c>
       <c r="C10" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/trainDataSet1.xml 7660</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/trainDataSet1.xml 14608</v>
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet1.xml 7660</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet1.xml 14608</v>
       </c>
       <c r="E10" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet2.xml 7660</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet2.xml 14608</v>
       </c>
       <c r="F10" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet3.xml 7660</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet3.xml 14608</v>
       </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet4.xml 7660</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet4.xml 14608</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
-        <v>15216</v>
+        <v>12612</v>
       </c>
       <c r="C11" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/trainDataSet1.xml 15216</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/trainDataSet1.xml 12612</v>
       </c>
       <c r="D11" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet1.xml 15216</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet1.xml 12612</v>
       </c>
       <c r="E11" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet2.xml 15216</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet2.xml 12612</v>
       </c>
       <c r="F11" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet3.xml 15216</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet3.xml 12612</v>
       </c>
       <c r="G11" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet4.xml 15216</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet4.xml 12612</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
-        <v>17384</v>
+        <v>13836</v>
       </c>
       <c r="C12" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/trainDataSet1.xml 17384</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/trainDataSet1.xml 13836</v>
       </c>
       <c r="D12" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet1.xml 17384</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet1.xml 13836</v>
       </c>
       <c r="E12" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet2.xml 17384</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet2.xml 13836</v>
       </c>
       <c r="F12" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet3.xml 17384</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet3.xml 13836</v>
       </c>
       <c r="G12" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet4.xml 17384</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet4.xml 13836</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
-        <v>8112</v>
+        <v>5936</v>
       </c>
       <c r="C13" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/trainDataSet1.xml 8112</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/trainDataSet1.xml 5936</v>
       </c>
       <c r="D13" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet1.xml 8112</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet1.xml 5936</v>
       </c>
       <c r="E13" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet2.xml 8112</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet2.xml 5936</v>
       </c>
       <c r="F13" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet3.xml 8112</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet3.xml 5936</v>
       </c>
       <c r="G13" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet4.xml 8112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
-        <v>16924</v>
-      </c>
-      <c r="C14" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/trainDataSet1.xml 16924</v>
-      </c>
-      <c r="D14" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet1.xml 16924</v>
-      </c>
-      <c r="E14" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet2.xml 16924</v>
-      </c>
-      <c r="F14" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet3.xml 16924</v>
-      </c>
-      <c r="G14" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet4.xml 16924</v>
+        <v>zzz Infer 32 Config/32/Client.xml Config/32/inferDataSet4.xml 5936</v>
       </c>
     </row>
   </sheetData>

</xml_diff>